<commit_message>
Implementation of code behind for AddNewCustomer Move of Collections from DataSetsClass to App.xaml and refactoring of code to work with new positon of Collections
</commit_message>
<xml_diff>
--- a/Projektplanering/To-do list.xlsx
+++ b/Projektplanering/To-do list.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="51">
   <si>
     <t>To-do list</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Implementera kod</t>
   </si>
   <si>
-    <t>Implemetation av funktionaliteten i CustomerViewn</t>
-  </si>
-  <si>
     <t>Code behind för att spara data</t>
   </si>
   <si>
@@ -225,6 +222,15 @@
   </si>
   <si>
     <t>Skapa vyn</t>
+  </si>
+  <si>
+    <t>Input validation</t>
+  </si>
+  <si>
+    <t>Saknar bara input validation</t>
+  </si>
+  <si>
+    <t>Göra knapp ej tryckbar om info saknas</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1067,7 @@
   <dimension ref="B1:E402"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1128,7 +1134,9 @@
       </c>
     </row>
     <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5"/>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
@@ -11630,7 +11638,7 @@
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="11"/>
     </row>
@@ -13735,7 +13743,7 @@
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="11"/>
     </row>
@@ -13779,7 +13787,7 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -15815,7 +15823,7 @@
   <dimension ref="B1:E402"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -15882,25 +15890,29 @@
       </c>
     </row>
     <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5"/>
+      <c r="B8" s="5">
+        <v>0.5</v>
+      </c>
       <c r="C8" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
+      <c r="B10" s="5"/>
       <c r="C10" t="s">
         <v>48</v>
       </c>
@@ -15909,7 +15921,9 @@
     </row>
     <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
-      <c r="C11"/>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="3"/>
     </row>

</xml_diff>